<commit_message>
Add fundamental user stories to the base documentation
</commit_message>
<xml_diff>
--- a/doc/cms_documentation.xlsx
+++ b/doc/cms_documentation.xlsx
@@ -8,36 +8,134 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CMS\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9097A6-7A06-47F0-8CBA-5833E3E4E35F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A13E6F-2D4F-436E-9E37-05B70897425B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Как" sheetId="1" r:id="rId1"/>
+    <sheet name="потребители" sheetId="3" r:id="rId2"/>
+    <sheet name="базова архитектура" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Архитектура</t>
-  </si>
-  <si>
-    <t>Приложение</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+  <si>
+    <t>Front-end разработка</t>
+  </si>
+  <si>
+    <t>*визуализация</t>
+  </si>
+  <si>
+    <t>*динамично разпределение на визуални компоненти</t>
+  </si>
+  <si>
+    <t>*процеса по комуникация със сървърите</t>
+  </si>
+  <si>
+    <t>технология</t>
+  </si>
+  <si>
+    <t>HTML / CSS / Java Script</t>
+  </si>
+  <si>
+    <t>Back-end</t>
+  </si>
+  <si>
+    <t>*архитектура на изчислителна система</t>
+  </si>
+  <si>
+    <t>*архитектура на база данни</t>
+  </si>
+  <si>
+    <t>*сервизи за комуникация с Front-end слой</t>
+  </si>
+  <si>
+    <t>PHP / MySQL</t>
+  </si>
+  <si>
+    <t>* Java / .NET / Python / Ruby / Go / Node JS</t>
+  </si>
+  <si>
+    <t>Страница за четене на блог постове</t>
+  </si>
+  <si>
+    <t>Всеки блог пост може да се чете самостоятелно</t>
+  </si>
+  <si>
+    <t>посетител</t>
+  </si>
+  <si>
+    <t>модератор</t>
+  </si>
+  <si>
+    <t>администратор</t>
+  </si>
+  <si>
+    <t>чете</t>
+  </si>
+  <si>
+    <t>създава съдържание</t>
+  </si>
+  <si>
+    <t>модифицира съществуващо съдържание</t>
+  </si>
+  <si>
+    <t>изтрива съдържание</t>
+  </si>
+  <si>
+    <t>права</t>
+  </si>
+  <si>
+    <t>роля</t>
+  </si>
+  <si>
+    <t>задача</t>
+  </si>
+  <si>
+    <t>роля която може да го вижда</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Административна страница за създаване на нови постове</t>
+  </si>
+  <si>
+    <t>модератор / администратор</t>
+  </si>
+  <si>
+    <t>Административна страница за създаване на нови категории блог постове</t>
+  </si>
+  <si>
+    <t>администратора</t>
+  </si>
+  <si>
+    <t>Административна страница за актуализация на съществуващи блог постове</t>
+  </si>
+  <si>
+    <t>Административна страница за изтриване на съществуващи блог постове</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +143,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,14 +199,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,28 +549,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:A7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDA5B9D-F767-4007-8D80-2722D6134B90}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB472E15-DF8F-420B-8A0E-6A7426FD6E60}">
+  <dimension ref="A3:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Authentication documentation section added
</commit_message>
<xml_diff>
--- a/doc/cms_documentation.xlsx
+++ b/doc/cms_documentation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CMS\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A13E6F-2D4F-436E-9E37-05B70897425B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911E2E9-E979-423C-BFAC-A32EB311B315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Как" sheetId="1" r:id="rId1"/>
     <sheet name="потребители" sheetId="3" r:id="rId2"/>
     <sheet name="базова архитектура" sheetId="2" r:id="rId3"/>
+    <sheet name="автентикация" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Front-end разработка</t>
   </si>
@@ -129,6 +130,36 @@
   </si>
   <si>
     <t>Административна страница за изтриване на съществуващи блог постове</t>
+  </si>
+  <si>
+    <t>Автентикация</t>
+  </si>
+  <si>
+    <t>Оторизация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sign in </t>
+  </si>
+  <si>
+    <t>sign up</t>
+  </si>
+  <si>
+    <t>методи за автентикация</t>
+  </si>
+  <si>
+    <t>вход ласически</t>
+  </si>
+  <si>
+    <t>дву факторна автентикация</t>
+  </si>
+  <si>
+    <t>сертификати / тоукъни</t>
   </si>
 </sst>
 </file>
@@ -244,13 +275,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,6 +295,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -626,7 +663,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,54 +675,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -701,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB472E15-DF8F-420B-8A0E-6A7426FD6E60}">
   <dimension ref="A3:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,93 +749,156 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2E9D7A-62F1-4D9C-9E9D-29BC55C05943}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>